<commit_message>
Latex - Implementacja finished, new elements in excel
</commit_message>
<xml_diff>
--- a/doc/excel/Statystyki.xlsx
+++ b/doc/excel/Statystyki.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nazwa nagrania</t>
   </si>
@@ -38,13 +38,16 @@
     <t>False positive</t>
   </si>
   <si>
-    <t>Wzorzec</t>
-  </si>
-  <si>
-    <t>ksiazka_x5_MK</t>
-  </si>
-  <si>
     <t>L.p.</t>
+  </si>
+  <si>
+    <t>wszystko_JP</t>
+  </si>
+  <si>
+    <t>Próg podobieństwa</t>
+  </si>
+  <si>
+    <t>wszystko_JP2</t>
   </si>
 </sst>
 </file>
@@ -403,12 +406,13 @@
   <dimension ref="A3:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
@@ -417,10 +421,10 @@
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -440,13 +444,21 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -454,10 +466,18 @@
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new test recordings and statistics
</commit_message>
<xml_diff>
--- a/doc/excel/Statystyki.xlsx
+++ b/doc/excel/Statystyki.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Nazwa nagrania</t>
   </si>
@@ -38,9 +38,6 @@
     <t>False positive</t>
   </si>
   <si>
-    <t>L.p.</t>
-  </si>
-  <si>
     <t>wszystko_JP</t>
   </si>
   <si>
@@ -48,6 +45,27 @@
   </si>
   <si>
     <t>wszystko_JP2</t>
+  </si>
+  <si>
+    <t>True positive [%]</t>
+  </si>
+  <si>
+    <t>fotel_x3_JP</t>
+  </si>
+  <si>
+    <t>ksiazka_x3_JP</t>
+  </si>
+  <si>
+    <t>Uwaga!</t>
+  </si>
+  <si>
+    <t>False positive wpisuję również, jeśli znaleziono słowo,</t>
+  </si>
+  <si>
+    <t>które nie występuje w nagraniu</t>
+  </si>
+  <si>
+    <t>krzeslo_x3_JP</t>
   </si>
 </sst>
 </file>
@@ -84,10 +102,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G23"/>
+  <dimension ref="A3:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,14 +438,14 @@
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -438,17 +459,21 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>0.85</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
         <v>4</v>
@@ -459,174 +484,261 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="G4" s="1">
+        <f>E4/D4*100</f>
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <f>E5/D5*100</f>
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6:G15" si="0">E6/D6*100</f>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1">
+      <c r="D14" s="2">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2">
         <v>2</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1">
+        <f>E14/D14*100</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1">
+        <f>E15/D15*100</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16:G18" si="1">E16/D16*100</f>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>15</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
+        <v>33.333333333333329</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>16</v>
-      </c>
+      <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -635,9 +747,7 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>17</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -646,9 +756,7 @@
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>18</v>
-      </c>
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -657,9 +765,7 @@
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>19</v>
-      </c>
+      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -678,5 +784,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>